<commit_message>
Complete Ch 05 03 Understanding circular dependencies
</commit_message>
<xml_diff>
--- a/Definitive Guide to DAX/DJ-2/05 Understanding CALCULATE and CALCULATETABLE/02 Understanding context transition/04 Context transition with measures/DJ.xlsx
+++ b/Definitive Guide to DAX/DJ-2/05 Understanding CALCULATE and CALCULATETABLE/02 Understanding context transition/04 Context transition with measures/DJ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github.com\open-word\DAX\Definitive Guide to DAX\DJ-2\05 Understanding CALCULATE and CALCULATETABLE\02 Understanding context transition\04 Context transition with measures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2282695-C254-4CD6-8BB6-1C0540607C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49495B5B-67B8-4778-AA22-F6642F562D06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21900" yWindow="3285" windowWidth="21600" windowHeight="11835" xr2:uid="{12C88C8F-1C63-41CB-B0F9-05321AAA7110}"/>
   </bookViews>
@@ -415,7 +415,7 @@
   <dimension ref="C3:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:F8"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>